<commit_message>
caso de uso vendas
</commit_message>
<xml_diff>
--- a/Particulares/Samuel/rastreamento.xlsx
+++ b/Particulares/Samuel/rastreamento.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Caracteristicas</t>
   </si>
@@ -87,13 +90,7 @@
     <t>Permite o operador cadastrar os tipos de serviços que a empresa ABrasil Express pode oferecer aos seus clientes.</t>
   </si>
   <si>
-    <t>Cadastro de valores de serviços prestados.</t>
-  </si>
-  <si>
     <t xml:space="preserve">SSSVEN03 </t>
-  </si>
-  <si>
-    <t>SSSVEN04 - SSSVEN05</t>
   </si>
   <si>
     <t>Valores diferenciados para cada região</t>
@@ -483,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,30 +513,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -558,78 +555,69 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1">
+    <sortState ref="A2:E8">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>